<commit_message>
done knownCard,need to investigate conditional formatting
</commit_message>
<xml_diff>
--- a/knownCard.xlsx
+++ b/knownCard.xlsx
@@ -8,12 +8,13 @@
     <sheet name="Position 13" sheetId="1" r:id="rId1"/>
     <sheet name="Position 24" sheetId="2" r:id="rId2"/>
     <sheet name="Position 5" sheetId="3" r:id="rId3"/>
+    <sheet name="Position 6" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t>Position 1,3</t>
   </si>
@@ -33,307 +34,400 @@
     <t>0</t>
   </si>
   <si>
-    <t>-0.0783235</t>
-  </si>
-  <si>
-    <t>0.0536128</t>
-  </si>
-  <si>
-    <t>-0.1909328</t>
+    <t>-0.0801513</t>
+  </si>
+  <si>
+    <t>0.0553868</t>
+  </si>
+  <si>
+    <t>-0.1938706</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>-0.0763833</t>
-  </si>
-  <si>
-    <t>0.0517457</t>
-  </si>
-  <si>
-    <t>-0.1820920</t>
+    <t>-0.0782869</t>
+  </si>
+  <si>
+    <t>0.0535960</t>
+  </si>
+  <si>
+    <t>-0.1841347</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>-0.0736438</t>
-  </si>
-  <si>
-    <t>0.0491037</t>
-  </si>
-  <si>
-    <t>-0.1716491</t>
+    <t>-0.0737754</t>
+  </si>
+  <si>
+    <t>0.0492273</t>
+  </si>
+  <si>
+    <t>-0.1733405</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>-0.0672454</t>
-  </si>
-  <si>
-    <t>0.0428752</t>
-  </si>
-  <si>
-    <t>-0.1680311</t>
+    <t>-0.0675318</t>
+  </si>
+  <si>
+    <t>0.0431692</t>
+  </si>
+  <si>
+    <t>-0.1627557</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>-0.0570715</t>
-  </si>
-  <si>
-    <t>0.0330665</t>
-  </si>
-  <si>
-    <t>-0.1281285</t>
+    <t>-0.0562174</t>
+  </si>
+  <si>
+    <t>0.0322409</t>
+  </si>
+  <si>
+    <t>-0.1255800</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>-0.0361752</t>
-  </si>
-  <si>
-    <t>0.0127373</t>
-  </si>
-  <si>
-    <t>-0.1120894</t>
+    <t>-0.0345669</t>
+  </si>
+  <si>
+    <t>0.0111647</t>
+  </si>
+  <si>
+    <t>-0.1136789</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
-    <t>0.0092888</t>
-  </si>
-  <si>
-    <t>-0.0313877</t>
-  </si>
-  <si>
-    <t>-0.0392086</t>
+    <t>0.0076911</t>
+  </si>
+  <si>
+    <t>-0.0298164</t>
+  </si>
+  <si>
+    <t>-0.0343315</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>0.0735185</t>
-  </si>
-  <si>
-    <t>-0.0939891</t>
-  </si>
-  <si>
-    <t>-0.0310782</t>
+    <t>0.0733518</t>
+  </si>
+  <si>
+    <t>-0.0938353</t>
+  </si>
+  <si>
+    <t>-0.0342207</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>0.1721912</t>
-  </si>
-  <si>
-    <t>-0.1904817</t>
-  </si>
-  <si>
-    <t>-0.1342955</t>
+    <t>0.1728711</t>
+  </si>
+  <si>
+    <t>-0.1911462</t>
+  </si>
+  <si>
+    <t>-0.1348992</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>0.2157261</t>
-  </si>
-  <si>
-    <t>-0.2329238</t>
-  </si>
-  <si>
-    <t>-0.1327111</t>
+    <t>0.2152953</t>
+  </si>
+  <si>
+    <t>-0.2325046</t>
+  </si>
+  <si>
+    <t>-0.1330256</t>
   </si>
   <si>
     <t>Position 2,4</t>
   </si>
   <si>
-    <t>0.0587128</t>
-  </si>
-  <si>
-    <t>-0.0799494</t>
-  </si>
-  <si>
-    <t>-0.1735798</t>
-  </si>
-  <si>
-    <t>0.0537427</t>
-  </si>
-  <si>
-    <t>-0.0750864</t>
-  </si>
-  <si>
-    <t>-0.1674126</t>
-  </si>
-  <si>
-    <t>0.0437403</t>
-  </si>
-  <si>
-    <t>-0.0653503</t>
-  </si>
-  <si>
-    <t>-0.1732503</t>
-  </si>
-  <si>
-    <t>0.0372892</t>
-  </si>
-  <si>
-    <t>-0.0590479</t>
-  </si>
-  <si>
-    <t>-0.1687272</t>
-  </si>
-  <si>
-    <t>0.0240220</t>
-  </si>
-  <si>
-    <t>-0.0460723</t>
-  </si>
-  <si>
-    <t>-0.1543068</t>
-  </si>
-  <si>
-    <t>-0.0019771</t>
-  </si>
-  <si>
-    <t>-0.0207230</t>
-  </si>
-  <si>
-    <t>-0.1542624</t>
-  </si>
-  <si>
-    <t>-0.0270396</t>
-  </si>
-  <si>
-    <t>0.0040271</t>
-  </si>
-  <si>
-    <t>-0.0411473</t>
-  </si>
-  <si>
-    <t>-0.0920645</t>
-  </si>
-  <si>
-    <t>0.0674453</t>
-  </si>
-  <si>
-    <t>-0.0343421</t>
-  </si>
-  <si>
-    <t>-0.1914423</t>
-  </si>
-  <si>
-    <t>0.1640577</t>
-  </si>
-  <si>
-    <t>-0.1354727</t>
-  </si>
-  <si>
-    <t>-0.2351249</t>
-  </si>
-  <si>
-    <t>0.2066381</t>
-  </si>
-  <si>
-    <t>-0.1391264</t>
+    <t>0.0580120</t>
+  </si>
+  <si>
+    <t>-0.0792576</t>
+  </si>
+  <si>
+    <t>-0.1705409</t>
+  </si>
+  <si>
+    <t>0.0509161</t>
+  </si>
+  <si>
+    <t>-0.0723407</t>
+  </si>
+  <si>
+    <t>-0.1710981</t>
+  </si>
+  <si>
+    <t>0.0437669</t>
+  </si>
+  <si>
+    <t>-0.0653708</t>
+  </si>
+  <si>
+    <t>-0.1713131</t>
+  </si>
+  <si>
+    <t>0.0368836</t>
+  </si>
+  <si>
+    <t>-0.0586552</t>
+  </si>
+  <si>
+    <t>-0.1697122</t>
+  </si>
+  <si>
+    <t>0.0245614</t>
+  </si>
+  <si>
+    <t>-0.0466039</t>
+  </si>
+  <si>
+    <t>-0.1563259</t>
+  </si>
+  <si>
+    <t>-0.0022668</t>
+  </si>
+  <si>
+    <t>-0.0204527</t>
+  </si>
+  <si>
+    <t>-0.1586107</t>
+  </si>
+  <si>
+    <t>-0.0275114</t>
+  </si>
+  <si>
+    <t>0.0044830</t>
+  </si>
+  <si>
+    <t>-0.0426319</t>
+  </si>
+  <si>
+    <t>-0.0931631</t>
+  </si>
+  <si>
+    <t>0.0685023</t>
+  </si>
+  <si>
+    <t>-0.0394403</t>
+  </si>
+  <si>
+    <t>-0.1925877</t>
+  </si>
+  <si>
+    <t>0.1651599</t>
+  </si>
+  <si>
+    <t>-0.1407477</t>
+  </si>
+  <si>
+    <t>-0.2350089</t>
+  </si>
+  <si>
+    <t>0.2065240</t>
+  </si>
+  <si>
+    <t>-0.1395015</t>
   </si>
   <si>
     <t>Position 5</t>
   </si>
   <si>
-    <t>-0.1540974</t>
-  </si>
-  <si>
-    <t>0.1276186</t>
-  </si>
-  <si>
-    <t>-0.2304334</t>
-  </si>
-  <si>
-    <t>-0.0604517</t>
-  </si>
-  <si>
-    <t>0.0366738</t>
-  </si>
-  <si>
-    <t>-0.1009406</t>
-  </si>
-  <si>
-    <t>0.0264154</t>
-  </si>
-  <si>
-    <t>-0.0476709</t>
-  </si>
-  <si>
-    <t>0.0253401</t>
-  </si>
-  <si>
-    <t>0.1088792</t>
-  </si>
-  <si>
-    <t>-0.1281472</t>
-  </si>
-  <si>
-    <t>-0.0013749</t>
-  </si>
-  <si>
-    <t>0.1835953</t>
-  </si>
-  <si>
-    <t>-0.2011052</t>
-  </si>
-  <si>
-    <t>-0.0408537</t>
-  </si>
-  <si>
-    <t>0.1396425</t>
-  </si>
-  <si>
-    <t>-0.1582149</t>
-  </si>
-  <si>
-    <t>-0.0278230</t>
-  </si>
-  <si>
-    <t>0.0919333</t>
-  </si>
-  <si>
-    <t>-0.1116452</t>
-  </si>
-  <si>
-    <t>-0.0086424</t>
-  </si>
-  <si>
-    <t>0.0423623</t>
-  </si>
-  <si>
-    <t>-0.0634311</t>
-  </si>
-  <si>
-    <t>-0.0510081</t>
-  </si>
-  <si>
-    <t>-0.0079633</t>
-  </si>
-  <si>
-    <t>-0.0152827</t>
-  </si>
-  <si>
-    <t>-0.3818566</t>
-  </si>
-  <si>
-    <t>-0.0614824</t>
-  </si>
-  <si>
-    <t>0.0370557</t>
-  </si>
-  <si>
-    <t>-0.3252513</t>
+    <t>-0.1544597</t>
+  </si>
+  <si>
+    <t>0.1279728</t>
+  </si>
+  <si>
+    <t>-0.2301272</t>
+  </si>
+  <si>
+    <t>-0.0591261</t>
+  </si>
+  <si>
+    <t>0.0353798</t>
+  </si>
+  <si>
+    <t>-0.1014980</t>
+  </si>
+  <si>
+    <t>0.0260365</t>
+  </si>
+  <si>
+    <t>-0.0473132</t>
+  </si>
+  <si>
+    <t>0.0210944</t>
+  </si>
+  <si>
+    <t>0.1069517</t>
+  </si>
+  <si>
+    <t>-0.1262644</t>
+  </si>
+  <si>
+    <t>-0.0000987</t>
+  </si>
+  <si>
+    <t>0.1831585</t>
+  </si>
+  <si>
+    <t>-0.2006729</t>
+  </si>
+  <si>
+    <t>-0.0385593</t>
+  </si>
+  <si>
+    <t>0.1372876</t>
+  </si>
+  <si>
+    <t>-0.1559223</t>
+  </si>
+  <si>
+    <t>-0.0290349</t>
+  </si>
+  <si>
+    <t>0.0904651</t>
+  </si>
+  <si>
+    <t>-0.1102048</t>
+  </si>
+  <si>
+    <t>-0.0054500</t>
+  </si>
+  <si>
+    <t>0.0425648</t>
+  </si>
+  <si>
+    <t>-0.0636326</t>
+  </si>
+  <si>
+    <t>-0.0524588</t>
+  </si>
+  <si>
+    <t>-0.0113663</t>
+  </si>
+  <si>
+    <t>-0.0119709</t>
+  </si>
+  <si>
+    <t>-0.3840469</t>
+  </si>
+  <si>
+    <t>-0.0598453</t>
+  </si>
+  <si>
+    <t>0.0354613</t>
+  </si>
+  <si>
+    <t>-0.3246187</t>
+  </si>
+  <si>
+    <t>Position 6</t>
+  </si>
+  <si>
+    <t>0.1314959</t>
+  </si>
+  <si>
+    <t>-0.1507123</t>
+  </si>
+  <si>
+    <t>-0.1094877</t>
+  </si>
+  <si>
+    <t>0.0577307</t>
+  </si>
+  <si>
+    <t>-0.0787615</t>
+  </si>
+  <si>
+    <t>-0.0987637</t>
+  </si>
+  <si>
+    <t>-0.0182230</t>
+  </si>
+  <si>
+    <t>-0.0046841</t>
+  </si>
+  <si>
+    <t>-0.0906327</t>
+  </si>
+  <si>
+    <t>-0.0935963</t>
+  </si>
+  <si>
+    <t>0.0687597</t>
+  </si>
+  <si>
+    <t>-0.1068902</t>
+  </si>
+  <si>
+    <t>-0.1456293</t>
+  </si>
+  <si>
+    <t>0.1194138</t>
+  </si>
+  <si>
+    <t>-0.1350319</t>
+  </si>
+  <si>
+    <t>-0.1722002</t>
+  </si>
+  <si>
+    <t>0.1452045</t>
+  </si>
+  <si>
+    <t>-0.1767399</t>
+  </si>
+  <si>
+    <t>-0.1710326</t>
+  </si>
+  <si>
+    <t>0.1439461</t>
+  </si>
+  <si>
+    <t>-0.2199294</t>
+  </si>
+  <si>
+    <t>-0.1112929</t>
+  </si>
+  <si>
+    <t>0.0857303</t>
+  </si>
+  <si>
+    <t>-0.2090100</t>
+  </si>
+  <si>
+    <t>-0.0458513</t>
+  </si>
+  <si>
+    <t>0.0219682</t>
+  </si>
+  <si>
+    <t>-0.1933530</t>
+  </si>
+  <si>
+    <t>0.0146350</t>
+  </si>
+  <si>
+    <t>-0.0369267</t>
+  </si>
+  <si>
+    <t>-0.1648497</t>
   </si>
 </sst>
 </file>
@@ -885,4 +979,176 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>